<commit_message>
saving changes to switch branch, contains 5-34 to 39 and 47
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_16.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_16.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="8_{FB6C5830-E429-CA47-B0D6-BBB99CFECB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46E7C19B-CF25-0D4E-9857-F7C4F3B54D4E}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="540" windowWidth="31000" windowHeight="16620" activeTab="1" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="42040" yWindow="720" windowWidth="31000" windowHeight="16620" activeTab="1" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -5879,9 +5879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEACD581-E79F-4912-9044-D35B08937AF8}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>